<commit_message>
create tag in tag case for testing
</commit_message>
<xml_diff>
--- a/SuppXLS/Scen_BND_PPFOSSIL.xlsx
+++ b/SuppXLS/Scen_BND_PPFOSSIL.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" mc:Ignorable="x15 xr xr6 xr10">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22730"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24326"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\VEDA\Training material\DemoS_012\SuppXLS\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Github\DemoS_012_testing_GitHub\SuppXLS\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{3A1C86BA-2C92-4E36-BB55-A28EA69C84D6}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E0F99D29-E454-4839-B341-AE9F83A561A4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1905" yWindow="1905" windowWidth="21600" windowHeight="11385" activeTab="2"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21390" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="INS" sheetId="2" r:id="rId1"/>
@@ -25,25 +25,17 @@
     <sheet name="Sheet9" sheetId="9" r:id="rId10"/>
   </sheets>
   <calcPr calcId="125725"/>
-  <extLst>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
-      </xcalcf:calcFeatures>
-    </ext>
-  </extLst>
 </workbook>
 </file>
 
 <file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
-<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
   <authors>
     <author>Maurizio Gargiulo</author>
     <author>Gary Goldstein</author>
   </authors>
   <commentList>
-    <comment ref="B2" authorId="0" shapeId="0">
+    <comment ref="B2" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000001000000}">
       <text>
         <r>
           <rPr>
@@ -57,7 +49,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="K2" authorId="1" shapeId="0">
+    <comment ref="K2" authorId="1" shapeId="0" xr:uid="{00000000-0006-0000-0000-000002000000}">
       <text>
         <r>
           <rPr>
@@ -70,7 +62,47 @@
         </r>
       </text>
     </comment>
-    <comment ref="P2" authorId="1" shapeId="0">
+    <comment ref="P2" authorId="1" shapeId="0" xr:uid="{00000000-0006-0000-0000-000003000000}">
+      <text>
+        <r>
+          <rPr>
+            <sz val="8"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Define the qualifiers based upon commodity set + name + descriptions, according to both include and exclude specifications.</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="C6" authorId="0" shapeId="0" xr:uid="{14CBE5E6-51D7-4D1A-BCDD-2959AB2A4BD5}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="8"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Insert Table</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="L6" authorId="1" shapeId="0" xr:uid="{33B72074-0045-4EC3-AFD9-F551701AF794}">
+      <text>
+        <r>
+          <rPr>
+            <sz val="8"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Define the qualifiers based upon technology set + topology + name + descriptions, according to both include and exclude specifications.</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="Q6" authorId="1" shapeId="0" xr:uid="{8359DB0D-B8A0-44F9-9A9D-DEE68430296B}">
       <text>
         <r>
           <rPr>
@@ -88,12 +120,12 @@
 </file>
 
 <file path=xl/comments2.xml><?xml version="1.0" encoding="utf-8"?>
-<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
   <authors>
     <author>Gary Goldstein</author>
   </authors>
   <commentList>
-    <comment ref="K2" authorId="0" shapeId="0">
+    <comment ref="K2" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0100-000001000000}">
       <text>
         <r>
           <rPr>
@@ -106,7 +138,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="P2" authorId="0" shapeId="0">
+    <comment ref="P2" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0100-000002000000}">
       <text>
         <r>
           <rPr>
@@ -124,7 +156,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="115" uniqueCount="44">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="137" uniqueCount="44">
   <si>
     <t>~UC_Sets: R_E: AllRegions</t>
   </si>
@@ -261,7 +293,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="9" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -410,8 +442,8 @@
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <cellStyle name="Normal 10" xfId="1"/>
-    <cellStyle name="Normale_Scen_UC_IND-StrucConst" xfId="2"/>
+    <cellStyle name="Normal 10" xfId="1" xr:uid="{00000000-0005-0000-0000-000001000000}"/>
+    <cellStyle name="Normale_Scen_UC_IND-StrucConst" xfId="2" xr:uid="{00000000-0005-0000-0000-000002000000}"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
@@ -746,11 +778,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:R4"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:S8"/>
   <sheetViews>
-    <sheetView topLeftCell="C1" zoomScale="180" zoomScaleNormal="180" workbookViewId="0">
-      <selection activeCell="C5" sqref="C5"/>
+    <sheetView tabSelected="1" zoomScale="180" zoomScaleNormal="180" workbookViewId="0">
+      <selection activeCell="C10" sqref="C10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -771,12 +803,12 @@
     <col min="17" max="18" width="8.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="2" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:19" x14ac:dyDescent="0.25">
       <c r="B2" s="9" t="s">
         <v>16</v>
       </c>
@@ -789,7 +821,7 @@
       <c r="Q2" s="11"/>
       <c r="R2" s="11"/>
     </row>
-    <row r="3" spans="1:18" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B3" s="12" t="s">
         <v>17</v>
       </c>
@@ -842,7 +874,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="4" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:19" x14ac:dyDescent="0.25">
       <c r="C4" t="s">
         <v>40</v>
       </c>
@@ -856,6 +888,94 @@
         <v>1000</v>
       </c>
       <c r="K4" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="5" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="B5" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="6" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="C6" s="9" t="s">
+        <v>16</v>
+      </c>
+      <c r="L6" s="10"/>
+      <c r="M6" s="11"/>
+      <c r="N6" s="11"/>
+      <c r="O6" s="11"/>
+      <c r="P6" s="11"/>
+      <c r="Q6" s="11"/>
+      <c r="R6" s="11"/>
+      <c r="S6" s="11"/>
+    </row>
+    <row r="7" spans="1:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C7" s="12" t="s">
+        <v>17</v>
+      </c>
+      <c r="D7" s="12" t="s">
+        <v>12</v>
+      </c>
+      <c r="E7" s="12" t="s">
+        <v>11</v>
+      </c>
+      <c r="F7" s="12" t="s">
+        <v>3</v>
+      </c>
+      <c r="G7" s="12" t="s">
+        <v>22</v>
+      </c>
+      <c r="H7" s="12" t="s">
+        <v>23</v>
+      </c>
+      <c r="I7" s="13" t="s">
+        <v>18</v>
+      </c>
+      <c r="J7" s="13" t="s">
+        <v>37</v>
+      </c>
+      <c r="K7" s="13" t="s">
+        <v>36</v>
+      </c>
+      <c r="L7" s="14" t="s">
+        <v>5</v>
+      </c>
+      <c r="M7" s="14" t="s">
+        <v>4</v>
+      </c>
+      <c r="N7" s="14" t="s">
+        <v>19</v>
+      </c>
+      <c r="O7" s="14" t="s">
+        <v>2</v>
+      </c>
+      <c r="P7" s="14" t="s">
+        <v>7</v>
+      </c>
+      <c r="Q7" s="14" t="s">
+        <v>20</v>
+      </c>
+      <c r="R7" s="14" t="s">
+        <v>6</v>
+      </c>
+      <c r="S7" s="14" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="8" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="D8" t="s">
+        <v>40</v>
+      </c>
+      <c r="E8" t="s">
+        <v>38</v>
+      </c>
+      <c r="F8">
+        <v>2020</v>
+      </c>
+      <c r="J8">
+        <v>1000</v>
+      </c>
+      <c r="L8" t="s">
         <v>39</v>
       </c>
     </row>
@@ -866,7 +986,7 @@
 </file>
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0900-000000000000}">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
@@ -878,7 +998,7 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:R3"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
@@ -979,10 +1099,10 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:N6"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" zoomScale="180" zoomScaleNormal="180" workbookViewId="0">
+    <sheetView zoomScale="180" zoomScaleNormal="180" workbookViewId="0">
       <selection activeCell="M15" sqref="M15"/>
     </sheetView>
   </sheetViews>
@@ -1081,7 +1201,7 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:O5"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
@@ -1163,7 +1283,7 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <dimension ref="A1:O5"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
@@ -1245,7 +1365,7 @@
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
   <dimension ref="A1:O5"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
@@ -1326,7 +1446,7 @@
 </file>
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -1340,7 +1460,7 @@
 </file>
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0700-000000000000}">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
@@ -1352,7 +1472,7 @@
 </file>
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0800-000000000000}">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>

</xml_diff>